<commit_message>
new Find page Element Create Client
</commit_message>
<xml_diff>
--- a/testData/testData.xlsx
+++ b/testData/testData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -50,15 +50,6 @@
     <t>a</t>
   </si>
   <si>
-    <t>LogIn Alis 1</t>
-  </si>
-  <si>
-    <t>LogIn Alis 2</t>
-  </si>
-  <si>
-    <t>a1</t>
-  </si>
-  <si>
     <t>LogIn Alis 3</t>
   </si>
   <si>
@@ -87,13 +78,25 @@
   </si>
   <si>
     <t>DataBase</t>
+  </si>
+  <si>
+    <t>http://alis-alf-app01:8080/af_pl_env1/alis1#alis</t>
+  </si>
+  <si>
+    <t>af_7000_defs</t>
+  </si>
+  <si>
+    <t>LogIn Alis TFL</t>
+  </si>
+  <si>
+    <t>LogIn Alis AF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,10 +105,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color rgb="FF6A8759"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -131,19 +142,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -459,36 +475,36 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>20</v>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -496,9 +512,9 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
@@ -508,7 +524,7 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -516,18 +532,18 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -536,19 +552,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -556,19 +572,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -576,19 +592,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
       <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
         <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -596,23 +612,26 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" location="alis" display="http://alis-alf-app01:8080/af_pl_env1/alis1 - alis"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>